<commit_message>
add new data pic
</commit_message>
<xml_diff>
--- a/final report/percisionRate_LSTM.xlsx
+++ b/final report/percisionRate_LSTM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanda/Documents/final Project/uki-uki-diasuki/final report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FILE\中正\大數據與資料分析\uki-uki-diasuki\final report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51022955-D6A9-9B49-AF4B-B41A62364431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2716A44D-4CD6-4AEB-BE39-DFF878CB3CBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="18735" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="percisionRate_LSTM" sheetId="1" r:id="rId1"/>
@@ -26,79 +26,53 @@
     <definedName name="_xlchart.v1.10" hidden="1">半導體!$G$2:$G$11</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">半導體!$H$1</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">半導體!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">半導體!$I$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">半導體!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">半導體!$B$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">半導體!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">半導體!$C$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">半導體!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">半導體!$G$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">半導體!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">半導體!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">半導體!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">半導體!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">半導體!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">半導體!$G$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">半導體!$G$2:$G$11</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">percisionRate_LSTM!$G$2:$G$41</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">半導體!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">半導體!$H$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">半導體!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">半導體!$I$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">半導體!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">半導體!$B$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">半導體!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">半導體!$C$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">半導體!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">半導體!$G$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">半導體!$H$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">半導體!$H$2:$H$11</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">半導體!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">食品!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">食品!$C$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">食品!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">食品!$G$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">食品!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">食品!$H$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">食品!$H$2:$H$11</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">percisionRate_LSTM!$H$2:$H$41</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">半導體!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">半導體!$H$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">半導體!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">半導體!$I$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">半導體!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">食品!$B$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">食品!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">食品!$C$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">食品!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">食品!$G$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">食品!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">航運!$B$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">航運!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">航運!$C$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">航運!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">航運!$G$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">航運!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">航運!$H$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">航運!$H$2:$H$11</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">航運!$I$2:$I$11</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">percisionRate_LSTM!$I$2:$I$41</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">食品!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">食品!$H$1</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">食品!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">食品!$I$1</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">食品!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">航運!$B$1</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">航運!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">航運!$C$1</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">航運!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">航運!$G$1</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">通訊!$B$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">通訊!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">通訊!$C$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">通訊!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">通訊!$G$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">通訊!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">通訊!$H$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">通訊!$H$2:$H$11</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">通訊!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">percisionRate_LSTM!$B$2:$B$41</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">半導體!$B$1</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">航運!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">航運!$H$1</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">航運!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">航運!$I$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">航運!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">航運!$B$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">航運!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">航運!$C$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">航運!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">航運!$G$1</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">percisionRate_LSTM!$C$2:$C$41</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">percisionRate_LSTM!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">percisionRate_LSTM!$H$2:$H$41</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">percisionRate_LSTM!$I$2:$I$41</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">半導體!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">航運!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">航運!$H$1</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">航運!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">航運!$I$1</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">航運!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">通訊!$B$1</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">通訊!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">通訊!$C$1</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">通訊!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">通訊!$G$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">半導體!$C$1</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">通訊!$G$2:$G$11</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">通訊!$H$1</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">通訊!$H$2:$H$11</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">通訊!$I$1</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">通訊!$I$2:$I$11</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">percisionRate_LSTM!$B$2:$B$41</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">percisionRate_LSTM!$C$2:$C$41</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">percisionRate_LSTM!$G$2:$G$41</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">percisionRate_LSTM!$H$2:$H$41</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">percisionRate_LSTM!$I$2:$I$41</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">半導體!$C$2:$C$11</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">半導體!$G$1</definedName>
   </definedNames>
@@ -110,8 +84,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -281,7 +255,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -289,7 +263,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -297,7 +271,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="major"/>
@@ -306,7 +280,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -315,7 +289,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -324,7 +298,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -332,7 +306,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -340,7 +314,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -348,7 +322,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -356,7 +330,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -365,7 +339,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -374,7 +348,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -382,7 +356,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -391,7 +365,7 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -399,7 +373,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -408,7 +382,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -417,7 +391,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -425,14 +399,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -440,7 +414,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF1E1E1E"/>
-      <name val="Calibri Light"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="major"/>
@@ -994,48 +968,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="中等" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="合計" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="計算方式" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="連結的儲存格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="備註" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="說明文字" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="輔色1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="輔色2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="輔色3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="輔色4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="輔色5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="輔色6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="標題" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="標題 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="標題 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標題 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="標題 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="輸入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="輸出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="檢查儲存格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="壞" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="警告文字" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1048,6 +1022,669 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>LSTM</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>統整!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>半導體</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>統整!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>q0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>統整!$B$33:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86749999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FCA-41C9-B4F7-5161B369F694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>統整!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>食品</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>統整!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>q0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>統整!$B$34:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85749999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6FCA-41C9-B4F7-5161B369F694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>統整!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>航運</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>統整!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>q0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>統整!$B$35:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87749999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6FCA-41C9-B4F7-5161B369F694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>統整!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>通訊</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>統整!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>q0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>統整!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86749999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6FCA-41C9-B4F7-5161B369F694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="500594016"/>
+        <c:axId val="465393312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="500594016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="465393312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="465393312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.91"/>
+          <c:min val="0.75000000000000011"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="500594016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1156,11 +1793,11 @@
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0">
-        <cx:catScaling gapWidth="1.5"/>
+        <cx:catScaling gapWidth="0.400000006"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling min="0.60000000000000009"/>
+        <cx:valScaling max="0.95000000000000007" min="0.60000000000000009"/>
         <cx:majorGridlines/>
         <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
@@ -1215,35 +1852,38 @@
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:rich>
-          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              </a:rPr>
-              <a:t>LSTM_半導體</a:t>
-            </a:r>
-          </a:p>
-        </cx:rich>
+        <cx:txData>
+          <cx:v>LSTM_半導體</cx:v>
+        </cx:txData>
       </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>LSTM_半導體</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
@@ -1302,6 +1942,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E7CDDDEC-7D22-D547-9812-B8D48771CA19}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>accuracy</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1321,6 +1962,25 @@
         <cx:majorGridlines/>
         <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="新細明體" panose="02020500000000000000" pitchFamily="18" charset="-120"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
     <cx:legend pos="r" align="ctr" overlay="0"/>
@@ -1333,27 +1993,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.40</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.42</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.44</cx:f>
+        <cx:f>_xlchart.v1.30</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1420,6 +2080,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{252A1A7E-B389-4643-A817-D3C2AC58AC1B}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>precision_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1432,7 +2093,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4D2653A5-79FA-2946-9F23-546C734B3D18}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.37</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>precision_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1445,7 +2106,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3B557D84-0E3D-3946-95ED-5CF3C33F5245}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.39</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>recall_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1458,7 +2119,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{710B2BB1-ED98-BA42-B1AE-8916D92123D1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.41</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>recall_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1471,6 +2132,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{63E60FCA-0C58-F64A-A9F0-640EF9F56CB3}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>accuracy</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1502,27 +2164,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.46</cx:f>
+        <cx:f>_xlchart.v1.32</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.48</cx:f>
+        <cx:f>_xlchart.v1.34</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.50</cx:f>
+        <cx:f>_xlchart.v1.36</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.38</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.54</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1573,7 +2235,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{548DB919-032B-5F4D-A062-8044F792EF25}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.45</cx:f>
+              <cx:f>_xlchart.v1.31</cx:f>
               <cx:v>precision_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1586,7 +2248,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{773F2198-2901-1440-8E78-FDC2A334E53F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.47</cx:f>
+              <cx:f>_xlchart.v1.33</cx:f>
               <cx:v>precision_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1599,7 +2261,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CFCC6B46-84CA-4A48-850C-3ED1CBC80EBF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.49</cx:f>
+              <cx:f>_xlchart.v1.35</cx:f>
               <cx:v>recall_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1612,7 +2274,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{ECCCDD7C-0FDA-8B4B-97A4-8BFA1BC24518}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.51</cx:f>
+              <cx:f>_xlchart.v1.37</cx:f>
               <cx:v>recall_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1625,6 +2287,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A48B1FCE-A69D-B845-8616-77EF612EDA0B}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>accuracy</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1656,27 +2319,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.66</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.68</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.70</cx:f>
+        <cx:f>_xlchart.v1.45</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.72</cx:f>
+        <cx:f>_xlchart.v1.47</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.74</cx:f>
+        <cx:f>_xlchart.v1.48</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1727,7 +2390,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{08E64D6D-FACE-4B40-8543-2F4DFAC167C2}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.65</cx:f>
+              <cx:f>_xlchart.v1.40</cx:f>
               <cx:v>precision_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1740,7 +2403,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{866C7E53-FE37-874F-A107-469768BA700D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.67</cx:f>
+              <cx:f>_xlchart.v1.42</cx:f>
               <cx:v>precision_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1753,7 +2416,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{812041D3-2B26-0947-8C7D-037165EA409B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.69</cx:f>
+              <cx:f>_xlchart.v1.44</cx:f>
               <cx:v>recall_0</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1766,7 +2429,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C23BC176-5B43-3F4D-90D8-BB048EA7EAC4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.71</cx:f>
+              <cx:f>_xlchart.v1.46</cx:f>
               <cx:v>recall_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1779,6 +2442,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{91FD20E2-73B8-374D-9385-F83027293C23}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>accuracy</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1810,27 +2474,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.75</cx:f>
+        <cx:f>_xlchart.v1.49</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.76</cx:f>
+        <cx:f>_xlchart.v1.50</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.77</cx:f>
+        <cx:f>_xlchart.v1.51</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.78</cx:f>
+        <cx:f>_xlchart.v1.52</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.53</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2213,6 +2877,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -5303,20 +6007,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>496956</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -5352,8 +6572,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4629150" y="9817100"/>
-              <a:ext cx="4908550" cy="3797300"/>
+              <a:off x="7737613" y="10440227"/>
+              <a:ext cx="4305300" cy="4079186"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5372,9 +6592,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5390,16 +6610,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>193675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -5435,8 +6655,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3956050" y="4318000"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7518400" y="3965575"/>
+              <a:ext cx="4572000" cy="2825750"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5455,9 +6675,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5518,8 +6738,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5302250" y="4406900"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="5324475" y="4540250"/>
+              <a:ext cx="4594225" cy="2832100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5538,9 +6758,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5601,8 +6821,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5302250" y="4406900"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="5324475" y="4543425"/>
+              <a:ext cx="4594225" cy="2832100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5621,9 +6841,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5684,8 +6904,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5302250" y="4406900"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="5324475" y="4540250"/>
+              <a:ext cx="4594225" cy="2832100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5704,9 +6924,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5767,8 +6987,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4787900" y="4191000"/>
-              <a:ext cx="5626100" cy="3467100"/>
+              <a:off x="4810125" y="4318000"/>
+              <a:ext cx="5651500" cy="3571875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5787,9 +7007,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+                <a:t>此圖表在您的 Excel 版本中無法使用。
+若編輯此圖案或將此活頁簿儲存為不同格式，將永久破壞圖表。</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5798,11 +7018,47 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>163995</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80133</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>2070</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99183</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16966DC-F508-4A10-80A7-67E68536BA73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6100,13 +7356,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" activeCellId="4" sqref="B2:B41 C2:C41 G2:G41 H2:H41 I2:I41"/>
+    <sheetView topLeftCell="C46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6180,7 +7436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1210</v>
       </c>
@@ -6254,7 +7510,7 @@
         <v>0.89336566817819396</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1215</v>
       </c>
@@ -6328,7 +7584,7 @@
         <v>1.0681358803472301</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1216</v>
       </c>
@@ -6402,7 +7658,7 @@
         <v>1.6176722274770501</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1218</v>
       </c>
@@ -6476,7 +7732,7 @@
         <v>0.71327594995691601</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1227</v>
       </c>
@@ -6550,7 +7806,7 @@
         <v>0.39148205687226201</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1229</v>
       </c>
@@ -6624,7 +7880,7 @@
         <v>0.82443222140133998</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1231</v>
       </c>
@@ -6698,7 +7954,7 @@
         <v>1.2900914483083299</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1232</v>
       </c>
@@ -6772,7 +8028,7 @@
         <v>3.8916377745197601</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1434</v>
       </c>
@@ -6846,7 +8102,7 @@
         <v>0.12965647004347899</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1702</v>
       </c>
@@ -6920,7 +8176,7 @@
         <v>0.821498383976491</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2330</v>
       </c>
@@ -6994,7 +8250,7 @@
         <v>13.4364318601646</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2337</v>
       </c>
@@ -7068,7 +8324,7 @@
         <v>1.28914500832087</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2344</v>
       </c>
@@ -7142,7 +8398,7 @@
         <v>1.2543159533594199</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2345</v>
       </c>
@@ -7216,7 +8472,7 @@
         <v>15.9432311334281</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2379</v>
       </c>
@@ -7290,7 +8546,7 @@
         <v>10.7280091340543</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2408</v>
       </c>
@@ -7364,7 +8620,7 @@
         <v>2.70934131895521</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>2412</v>
       </c>
@@ -7438,7 +8694,7 @@
         <v>0.98241955736776299</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2412</v>
       </c>
@@ -7512,7 +8768,7 @@
         <v>0.75389626094613404</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2439</v>
       </c>
@@ -7586,7 +8842,7 @@
         <v>1.6297600800638301</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2449</v>
       </c>
@@ -7660,7 +8916,7 @@
         <v>1.2759571299155601</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2454</v>
       </c>
@@ -7734,7 +8990,7 @@
         <v>15.387795478179999</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2455</v>
       </c>
@@ -7808,7 +9064,7 @@
         <v>2.2357615178842098</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>2459</v>
       </c>
@@ -7882,7 +9138,7 @@
         <v>0.58644450286531902</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2468</v>
       </c>
@@ -7956,7 +9212,7 @@
         <v>0.11807803502896901</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2498</v>
       </c>
@@ -8030,7 +9286,7 @@
         <v>2.70524605277163</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>2603</v>
       </c>
@@ -8104,7 +9360,7 @@
         <v>5.1380889813349002</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>2607</v>
       </c>
@@ -8178,7 +9434,7 @@
         <v>1.1615376573112</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>2609</v>
       </c>
@@ -8252,7 +9508,7 @@
         <v>7.1666028267344997</v>
       </c>
     </row>
-    <row r="30" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>2610</v>
       </c>
@@ -8326,7 +9582,7 @@
         <v>0.48741371294102098</v>
       </c>
     </row>
-    <row r="31" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>2615</v>
       </c>
@@ -8400,7 +9656,7 @@
         <v>14.7031666659525</v>
       </c>
     </row>
-    <row r="32" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>2618</v>
       </c>
@@ -8474,7 +9730,7 @@
         <v>0.74186538628795595</v>
       </c>
     </row>
-    <row r="33" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>2633</v>
       </c>
@@ -8548,7 +9804,7 @@
         <v>0.13082149662731099</v>
       </c>
     </row>
-    <row r="34" spans="1:24" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>2634</v>
       </c>
@@ -8622,7 +9878,7 @@
         <v>0.200369124804887</v>
       </c>
     </row>
-    <row r="35" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>2637</v>
       </c>
@@ -8696,7 +9952,7 @@
         <v>4.7769234417835698</v>
       </c>
     </row>
-    <row r="36" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>3034</v>
       </c>
@@ -8770,7 +10026,7 @@
         <v>15.6109997118932</v>
       </c>
     </row>
-    <row r="37" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>3035</v>
       </c>
@@ -8844,7 +10100,7 @@
         <v>5.75726658864368</v>
       </c>
     </row>
-    <row r="38" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>3045</v>
       </c>
@@ -8918,7 +10174,7 @@
         <v>0.41898897108095001</v>
       </c>
     </row>
-    <row r="39" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>3596</v>
       </c>
@@ -8992,7 +10248,7 @@
         <v>1.8160621294492501</v>
       </c>
     </row>
-    <row r="40" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>3682</v>
       </c>
@@ -9066,7 +10322,7 @@
         <v>0.155431466589703</v>
       </c>
     </row>
-    <row r="41" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>4904</v>
       </c>
@@ -9140,7 +10396,7 @@
         <v>0.18729192471008499</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -9237,7 +10493,7 @@
         <v>0.11807803502896901</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -9334,7 +10590,7 @@
         <v>0.68156808818401671</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -9431,7 +10687,7 @@
         <v>1.26513654163749</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -9528,7 +10784,7 @@
         <v>4.1129591913357126</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -9625,7 +10881,7 @@
         <v>15.9432311334281</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -9722,7 +10978,7 @@
         <v>4.9106454137313671</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>1</v>
       </c>
@@ -9739,7 +10995,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -9760,7 +11016,7 @@
       </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -9781,7 +11037,7 @@
       </c>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>27</v>
       </c>
@@ -9802,7 +11058,7 @@
       </c>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -9823,7 +11079,7 @@
       </c>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -9844,7 +11100,7 @@
       </c>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>5.583342900872016E-2</v>
       </c>
@@ -9873,16 +11129,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -9956,7 +11212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>2330</v>
       </c>
@@ -10030,7 +11286,7 @@
         <v>13.4364318601646</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2337</v>
       </c>
@@ -10104,7 +11360,7 @@
         <v>1.28914500832087</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2344</v>
       </c>
@@ -10178,7 +11434,7 @@
         <v>1.2543159533594199</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2379</v>
       </c>
@@ -10252,7 +11508,7 @@
         <v>10.7280091340543</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2408</v>
       </c>
@@ -10326,7 +11582,7 @@
         <v>2.70934131895521</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2449</v>
       </c>
@@ -10400,7 +11656,7 @@
         <v>1.2759571299155601</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>2454</v>
       </c>
@@ -10474,7 +11730,7 @@
         <v>15.387795478179999</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>2468</v>
       </c>
@@ -10548,7 +11804,7 @@
         <v>0.11807803502896901</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>3034</v>
       </c>
@@ -10622,7 +11878,7 @@
         <v>15.6109997118932</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>3035</v>
       </c>
@@ -10696,7 +11952,7 @@
         <v>5.75726658864368</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -10793,7 +12049,7 @@
         <v>0.11807803502896901</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -10890,7 +12146,7 @@
         <v>1.2792540995168875</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -10987,7 +12243,7 @@
         <v>4.233303953799445</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -11084,7 +12340,7 @@
         <v>12.759326178637025</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -11181,7 +12437,7 @@
         <v>15.6109997118932</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -11293,9 +12549,9 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -11369,7 +12625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1210</v>
       </c>
@@ -11443,7 +12699,7 @@
         <v>0.89336566817819396</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1215</v>
       </c>
@@ -11517,7 +12773,7 @@
         <v>1.0681358803472301</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1216</v>
       </c>
@@ -11591,7 +12847,7 @@
         <v>1.6176722274770501</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1218</v>
       </c>
@@ -11665,7 +12921,7 @@
         <v>0.71327594995691601</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1227</v>
       </c>
@@ -11739,7 +12995,7 @@
         <v>0.39148205687226201</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1229</v>
       </c>
@@ -11813,7 +13069,7 @@
         <v>0.82443222140133998</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1231</v>
       </c>
@@ -11887,7 +13143,7 @@
         <v>1.2900914483083299</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1232</v>
       </c>
@@ -11961,7 +13217,7 @@
         <v>3.8916377745197601</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>1434</v>
       </c>
@@ -12035,7 +13291,7 @@
         <v>0.12965647004347899</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>1702</v>
       </c>
@@ -12109,7 +13365,7 @@
         <v>0.821498383976491</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -12206,7 +13462,7 @@
         <v>0.12965647004347899</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -12303,7 +13559,7 @@
         <v>0.74033155846180976</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -12400,7 +13656,7 @@
         <v>0.85889894478976703</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -12497,7 +13753,7 @@
         <v>1.2346025563180549</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -12594,7 +13850,7 @@
         <v>3.8916377745197601</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -12706,9 +13962,9 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -12782,7 +14038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>2459</v>
       </c>
@@ -12856,7 +14112,7 @@
         <v>0.58644450286531902</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2603</v>
       </c>
@@ -12930,7 +14186,7 @@
         <v>5.1380889813349002</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2607</v>
       </c>
@@ -13004,7 +14260,7 @@
         <v>1.1615376573112</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2609</v>
       </c>
@@ -13078,7 +14334,7 @@
         <v>7.1666028267344997</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2610</v>
       </c>
@@ -13152,7 +14408,7 @@
         <v>0.48741371294102098</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2615</v>
       </c>
@@ -13226,7 +14482,7 @@
         <v>14.7031666659525</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>2618</v>
       </c>
@@ -13300,7 +14556,7 @@
         <v>0.74186538628795595</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>2633</v>
       </c>
@@ -13374,7 +14630,7 @@
         <v>0.13082149662731099</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2634</v>
       </c>
@@ -13448,7 +14704,7 @@
         <v>0.200369124804887</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2637</v>
       </c>
@@ -13522,7 +14778,7 @@
         <v>4.7769234417835698</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -13619,7 +14875,7 @@
         <v>0.13082149662731099</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -13716,7 +14972,7 @@
         <v>0.51217141042209546</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -13813,7 +15069,7 @@
         <v>0.9517015217995779</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -13910,7 +15166,7 @@
         <v>5.0477975964470678</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -14007,7 +15263,7 @@
         <v>14.7031666659525</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -14119,9 +15375,9 @@
       <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -14195,7 +15451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>2345</v>
       </c>
@@ -14269,7 +15525,7 @@
         <v>15.9432311334281</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2412</v>
       </c>
@@ -14343,7 +15599,7 @@
         <v>0.98241955736776299</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2412</v>
       </c>
@@ -14417,7 +15673,7 @@
         <v>0.75389626094613404</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2439</v>
       </c>
@@ -14491,7 +15747,7 @@
         <v>1.6297600800638301</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2455</v>
       </c>
@@ -14565,7 +15821,7 @@
         <v>2.2357615178842098</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2498</v>
       </c>
@@ -14639,7 +15895,7 @@
         <v>2.70524605277163</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>3045</v>
       </c>
@@ -14713,7 +15969,7 @@
         <v>0.41898897108095001</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>3596</v>
       </c>
@@ -14787,7 +16043,7 @@
         <v>1.8160621294492501</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>3682</v>
       </c>
@@ -14861,7 +16117,7 @@
         <v>0.155431466589703</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>4904</v>
       </c>
@@ -14935,7 +16191,7 @@
         <v>0.18729192471008499</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -15032,7 +16288,7 @@
         <v>0.155431466589703</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -15129,7 +16385,7 @@
         <v>0.50271579354724605</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -15226,7 +16482,7 @@
         <v>1.3060898187157965</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -15323,7 +16579,7 @@
         <v>2.1308366707754698</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -15420,7 +16676,7 @@
         <v>15.9432311334281</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -15528,13 +16784,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15608,7 +16864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -15682,7 +16938,7 @@
         <v>4.233303953799445</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -15756,7 +17012,7 @@
         <v>0.85889894478976703</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -15830,7 +17086,7 @@
         <v>0.9517015217995779</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -15904,7 +17160,7 @@
         <v>1.3060898187157965</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>38</v>
       </c>
@@ -15922,7 +17178,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>36</v>
@@ -15956,7 +17212,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>32</v>
       </c>
@@ -16004,7 +17260,7 @@
         <v>15.6109997118932</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -16052,7 +17308,7 @@
         <v>3.8916377745197601</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -16100,7 +17356,7 @@
         <v>14.7031666659525</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
@@ -16148,7 +17404,7 @@
         <v>15.9432311334281</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>39</v>
       </c>
@@ -16158,7 +17414,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>36</v>
@@ -16192,7 +17448,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
@@ -16235,7 +17491,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
@@ -16278,7 +17534,7 @@
         <v>0.8175</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
@@ -16321,7 +17577,7 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -16364,7 +17620,7 @@
         <v>0.86250000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>41</v>
       </c>
@@ -16392,7 +17648,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
         <v>36</v>
@@ -16410,7 +17666,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
@@ -16435,7 +17691,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>33</v>
       </c>
@@ -16460,7 +17716,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>34</v>
       </c>
@@ -16485,7 +17741,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
@@ -16510,7 +17766,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>40</v>
       </c>
@@ -16520,7 +17776,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7" t="s">
         <v>36</v>
@@ -16538,7 +17794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
@@ -16563,7 +17819,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>33</v>
       </c>
@@ -16588,7 +17844,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>34</v>
       </c>
@@ -16613,7 +17869,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>35</v>
       </c>
@@ -16638,7 +17894,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>42</v>
       </c>
@@ -16648,7 +17904,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7" t="s">
         <v>36</v>
@@ -16666,7 +17922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>32</v>
       </c>
@@ -16691,7 +17947,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>33</v>
       </c>
@@ -16716,7 +17972,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>34</v>
       </c>
@@ -16741,7 +17997,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
@@ -16766,7 +18022,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>43</v>
       </c>
@@ -16776,7 +18032,7 @@
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7" t="s">
         <v>36</v>
@@ -16794,7 +18050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>32</v>
       </c>
@@ -16819,7 +18075,7 @@
         <v>15.6109997118932</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>33</v>
       </c>
@@ -16844,7 +18100,7 @@
         <v>3.8916377745197601</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>34</v>
       </c>
@@ -16869,7 +18125,7 @@
         <v>14.7031666659525</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>35</v>
       </c>

</xml_diff>